<commit_message>
give this a look!!
</commit_message>
<xml_diff>
--- a/outputs/Moments.xlsx
+++ b/outputs/Moments.xlsx
@@ -488,16 +488,16 @@
         <v>6.25</v>
       </c>
       <c r="C3" t="n">
-        <v>26772.94921875001</v>
+        <v>32892.48046875001</v>
       </c>
       <c r="D3" t="n">
-        <v>1777.34375</v>
+        <v>2183.59375</v>
       </c>
       <c r="E3" t="n">
-        <v>1173.046875</v>
+        <v>1441.171875</v>
       </c>
       <c r="F3" t="n">
-        <v>820.3125</v>
+        <v>694.5902301087816</v>
       </c>
     </row>
     <row r="4">
@@ -508,16 +508,16 @@
         <v>12.5</v>
       </c>
       <c r="C4" t="n">
-        <v>45896.48437500001</v>
+        <v>58135.54687500001</v>
       </c>
       <c r="D4" t="n">
-        <v>3046.875</v>
+        <v>3859.375</v>
       </c>
       <c r="E4" t="n">
-        <v>2010.9375</v>
+        <v>2547.1875</v>
       </c>
       <c r="F4" t="n">
-        <v>1406.25</v>
+        <v>1227.647848564358</v>
       </c>
     </row>
     <row r="5">
@@ -528,16 +528,16 @@
         <v>18.75</v>
       </c>
       <c r="C5" t="n">
-        <v>57370.60546875001</v>
+        <v>75729.19921875001</v>
       </c>
       <c r="D5" t="n">
-        <v>3808.59375</v>
+        <v>5027.34375</v>
       </c>
       <c r="E5" t="n">
-        <v>2513.671875</v>
+        <v>3318.046875</v>
       </c>
       <c r="F5" t="n">
-        <v>1757.8125</v>
+        <v>1599.17285536673</v>
       </c>
     </row>
     <row r="6">
@@ -548,16 +548,16 @@
         <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>61195.31250000001</v>
+        <v>85673.43750000001</v>
       </c>
       <c r="D6" t="n">
-        <v>4062.5</v>
+        <v>5687.5</v>
       </c>
       <c r="E6" t="n">
-        <v>2681.25</v>
+        <v>3753.75</v>
       </c>
       <c r="F6" t="n">
-        <v>1875</v>
+        <v>1809.165250515896</v>
       </c>
     </row>
     <row r="7">
@@ -568,16 +568,16 @@
         <v>31.25</v>
       </c>
       <c r="C7" t="n">
-        <v>57370.60546875001</v>
+        <v>87968.26171875001</v>
       </c>
       <c r="D7" t="n">
-        <v>3808.59375</v>
+        <v>5839.84375</v>
       </c>
       <c r="E7" t="n">
-        <v>2513.671875</v>
+        <v>3854.296875</v>
       </c>
       <c r="F7" t="n">
-        <v>1757.8125</v>
+        <v>1857.625034011858</v>
       </c>
     </row>
     <row r="8">
@@ -588,16 +588,16 @@
         <v>37.5</v>
       </c>
       <c r="C8" t="n">
-        <v>45896.48437500001</v>
+        <v>82613.67187500001</v>
       </c>
       <c r="D8" t="n">
-        <v>3046.875</v>
+        <v>5484.375</v>
       </c>
       <c r="E8" t="n">
-        <v>2010.9375</v>
+        <v>3619.6875</v>
       </c>
       <c r="F8" t="n">
-        <v>1406.25</v>
+        <v>1744.552205854614</v>
       </c>
     </row>
     <row r="9">
@@ -608,16 +608,16 @@
         <v>43.75</v>
       </c>
       <c r="C9" t="n">
-        <v>26772.94921875001</v>
+        <v>69609.66796875001</v>
       </c>
       <c r="D9" t="n">
-        <v>1777.34375</v>
+        <v>4621.09375</v>
       </c>
       <c r="E9" t="n">
-        <v>1173.046875</v>
+        <v>3049.921875</v>
       </c>
       <c r="F9" t="n">
-        <v>820.3125</v>
+        <v>1469.946766044166</v>
       </c>
     </row>
     <row r="10">
@@ -628,16 +628,16 @@
         <v>50</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>48956.25000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>3250</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>2145</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>1033.808714580512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dead load reactions calculations
</commit_message>
<xml_diff>
--- a/outputs/Moments.xlsx
+++ b/outputs/Moments.xlsx
@@ -488,16 +488,16 @@
         <v>6.25</v>
       </c>
       <c r="C3" t="n">
-        <v>32892.48046875001</v>
+        <v>26772.94921875001</v>
       </c>
       <c r="D3" t="n">
-        <v>2183.59375</v>
+        <v>1777.34375</v>
       </c>
       <c r="E3" t="n">
-        <v>1441.171875</v>
+        <v>1173.046875</v>
       </c>
       <c r="F3" t="n">
-        <v>694.5902301087816</v>
+        <v>820.3125</v>
       </c>
     </row>
     <row r="4">
@@ -508,16 +508,16 @@
         <v>12.5</v>
       </c>
       <c r="C4" t="n">
-        <v>58135.54687500001</v>
+        <v>45896.48437500001</v>
       </c>
       <c r="D4" t="n">
-        <v>3859.375</v>
+        <v>3046.875</v>
       </c>
       <c r="E4" t="n">
-        <v>2547.1875</v>
+        <v>2010.9375</v>
       </c>
       <c r="F4" t="n">
-        <v>1227.647848564358</v>
+        <v>1406.25</v>
       </c>
     </row>
     <row r="5">
@@ -528,16 +528,16 @@
         <v>18.75</v>
       </c>
       <c r="C5" t="n">
-        <v>75729.19921875001</v>
+        <v>57370.60546875001</v>
       </c>
       <c r="D5" t="n">
-        <v>5027.34375</v>
+        <v>3808.59375</v>
       </c>
       <c r="E5" t="n">
-        <v>3318.046875</v>
+        <v>2513.671875</v>
       </c>
       <c r="F5" t="n">
-        <v>1599.17285536673</v>
+        <v>1757.8125</v>
       </c>
     </row>
     <row r="6">
@@ -548,16 +548,16 @@
         <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>85673.43750000001</v>
+        <v>61195.31250000001</v>
       </c>
       <c r="D6" t="n">
-        <v>5687.5</v>
+        <v>4062.5</v>
       </c>
       <c r="E6" t="n">
-        <v>3753.75</v>
+        <v>2681.25</v>
       </c>
       <c r="F6" t="n">
-        <v>1809.165250515896</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="7">
@@ -568,16 +568,16 @@
         <v>31.25</v>
       </c>
       <c r="C7" t="n">
-        <v>87968.26171875001</v>
+        <v>57370.60546875001</v>
       </c>
       <c r="D7" t="n">
-        <v>5839.84375</v>
+        <v>3808.59375</v>
       </c>
       <c r="E7" t="n">
-        <v>3854.296875</v>
+        <v>2513.671875</v>
       </c>
       <c r="F7" t="n">
-        <v>1857.625034011858</v>
+        <v>1757.8125</v>
       </c>
     </row>
     <row r="8">
@@ -588,16 +588,16 @@
         <v>37.5</v>
       </c>
       <c r="C8" t="n">
-        <v>82613.67187500001</v>
+        <v>45896.48437500001</v>
       </c>
       <c r="D8" t="n">
-        <v>5484.375</v>
+        <v>3046.875</v>
       </c>
       <c r="E8" t="n">
-        <v>3619.6875</v>
+        <v>2010.9375</v>
       </c>
       <c r="F8" t="n">
-        <v>1744.552205854614</v>
+        <v>1406.25</v>
       </c>
     </row>
     <row r="9">
@@ -608,16 +608,16 @@
         <v>43.75</v>
       </c>
       <c r="C9" t="n">
-        <v>69609.66796875001</v>
+        <v>26772.94921875001</v>
       </c>
       <c r="D9" t="n">
-        <v>4621.09375</v>
+        <v>1777.34375</v>
       </c>
       <c r="E9" t="n">
-        <v>3049.921875</v>
+        <v>1173.046875</v>
       </c>
       <c r="F9" t="n">
-        <v>1469.946766044166</v>
+        <v>820.3125</v>
       </c>
     </row>
     <row r="10">
@@ -628,16 +628,16 @@
         <v>50</v>
       </c>
       <c r="C10" t="n">
-        <v>48956.25000000001</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>3250</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>2145</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>1033.808714580512</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>